<commit_message>
Update Test Data Path
</commit_message>
<xml_diff>
--- a/Test Data/MasterInput.xlsx
+++ b/Test Data/MasterInput.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MBF_Documents\fintegrity-katalon2\Test Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="750" windowWidth="19875" windowHeight="6840"/>
+    <workbookView xWindow="480" yWindow="750" windowWidth="19875" windowHeight="6840" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="EntryBooking" sheetId="2" r:id="rId1"/>
@@ -20,12 +15,12 @@
     <sheet name="UpdateAdditionalInfo" sheetId="3" r:id="rId6"/>
     <sheet name="FacilityTermination" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
   <si>
     <t>CustomerName</t>
   </si>
@@ -129,12 +124,6 @@
     <t>NewContract_CC01 UAI</t>
   </si>
   <si>
-    <t>DIYAS</t>
-  </si>
-  <si>
-    <t>YOMMIE</t>
-  </si>
-  <si>
     <t>Maker</t>
   </si>
   <si>
@@ -223,6 +212,9 @@
   </si>
   <si>
     <t>abcde SUDIRMAN</t>
+  </si>
+  <si>
+    <t>KALEB</t>
   </si>
 </sst>
 </file>
@@ -332,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,7 +359,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -578,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -593,13 +585,13 @@
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>0</v>
@@ -631,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
@@ -646,7 +638,7 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -717,7 +709,7 @@
         <v>DADANG KONELO</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
@@ -783,7 +775,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -792,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" t="str">
         <f>EntryBooking!D2</f>
@@ -877,37 +869,37 @@
         <v>10</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -915,10 +907,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -939,13 +931,13 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K2">
         <v>3275112405840000</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M2">
         <v>3172000000</v>
@@ -957,13 +949,13 @@
         <v>3172011005</v>
       </c>
       <c r="P2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" t="s">
         <v>59</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>60</v>
-      </c>
-      <c r="R2" t="s">
-        <v>61</v>
       </c>
       <c r="S2">
         <v>81123456789</v>
@@ -978,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,10 +1020,10 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
         <v>31</v>
@@ -1126,30 +1118,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change CA User Facility Register to Suharno
</commit_message>
<xml_diff>
--- a/Test Data/MasterInput.xlsx
+++ b/Test Data/MasterInput.xlsx
@@ -214,7 +214,7 @@
     <t>abcde SUDIRMAN</t>
   </si>
   <si>
-    <t>KALEB</t>
+    <t>SUHARNO</t>
   </si>
 </sst>
 </file>
@@ -971,7 +971,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Quality Checkpoint Test Suite - Test Data/MasterInput.xlsx for upinfo and disbursement
</commit_message>
<xml_diff>
--- a/Test Data/MasterInput.xlsx
+++ b/Test Data/MasterInput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="750" windowWidth="19875" windowHeight="6840" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="810" windowWidth="19875" windowHeight="6780" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="EntryBooking" sheetId="2" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="FacilityRegister" sheetId="5" r:id="rId5"/>
     <sheet name="UpdateAdditionalInfo" sheetId="3" r:id="rId6"/>
     <sheet name="FacilityTermination" sheetId="8" r:id="rId7"/>
+    <sheet name="Disbursement" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
   <si>
     <t>CustomerName</t>
   </si>
@@ -215,13 +216,28 @@
   </si>
   <si>
     <t>SUHARNO</t>
+  </si>
+  <si>
+    <t>FINMaker</t>
+  </si>
+  <si>
+    <t>FINChecker</t>
+  </si>
+  <si>
+    <t>FINDir</t>
+  </si>
+  <si>
+    <t>RACHMITA</t>
+  </si>
+  <si>
+    <t>HIROSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +249,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -258,12 +281,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,7 +994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1039,7 +1063,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,4 +1171,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="str">
+        <f>'CDB Personal'!E2</f>
+        <v>DADANG KONELO</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Facility Test Suite
</commit_message>
<xml_diff>
--- a/Test Data/MasterInput.xlsx
+++ b/Test Data/MasterInput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="810" windowWidth="19875" windowHeight="6780" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="810" windowWidth="19875" windowHeight="6780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EntryBooking" sheetId="2" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t>YANUAR</t>
   </si>
   <si>
-    <t>123123193868</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>HIROSE</t>
+  </si>
+  <si>
+    <t>123123193132</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>19</v>
@@ -662,7 +662,7 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,7 +733,7 @@
         <v>DADANG KONELO</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>27</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -893,37 +893,37 @@
         <v>10</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -934,7 +934,7 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -955,13 +955,13 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K2">
         <v>3275112405840000</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M2">
         <v>3172000000</v>
@@ -973,13 +973,13 @@
         <v>3172011005</v>
       </c>
       <c r="P2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>58</v>
-      </c>
-      <c r="R2" t="s">
-        <v>59</v>
       </c>
       <c r="S2">
         <v>81123456789</v>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -1148,24 +1148,24 @@
         <v>35</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1177,7 +1177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1199,13 +1199,13 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1220,13 +1220,13 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Term Sim Test Suite
</commit_message>
<xml_diff>
--- a/Test Data/MasterInput.xlsx
+++ b/Test Data/MasterInput.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="810" windowWidth="19875" windowHeight="6780" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="810" windowWidth="19875" windowHeight="6780" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="EntryBooking" sheetId="2" r:id="rId1"/>
@@ -13,15 +13,16 @@
     <sheet name="CDB RO" sheetId="9" r:id="rId4"/>
     <sheet name="FacilityRegister" sheetId="5" r:id="rId5"/>
     <sheet name="UpdateAdditionalInfo" sheetId="3" r:id="rId6"/>
-    <sheet name="FacilityTermination" sheetId="8" r:id="rId7"/>
-    <sheet name="Disbursement" sheetId="11" r:id="rId8"/>
+    <sheet name="Facility Termination Simulation" sheetId="12" r:id="rId7"/>
+    <sheet name="FacilityTermination" sheetId="8" r:id="rId8"/>
+    <sheet name="Disbursement" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>CustomerName</t>
   </si>
@@ -231,6 +232,15 @@
   </si>
   <si>
     <t>123123193132</t>
+  </si>
+  <si>
+    <t>YUNILIA</t>
+  </si>
+  <si>
+    <t>TermSimMaker</t>
+  </si>
+  <si>
+    <t>TermSimChecker</t>
   </si>
 </sst>
 </file>
@@ -675,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -995,7 +1005,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1073,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,6 +1137,49 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="str">
+        <f>EntryBooking!D2</f>
+        <v>DADANG KONELO</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1173,12 +1226,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1276,7 @@
         <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
         <v>68</v>

</xml_diff>